<commit_message>
ENH: Loading and checking for demographics
</commit_message>
<xml_diff>
--- a/tests/test_data_measurement/demographics.xlsx
+++ b/tests/test_data_measurement/demographics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="5680" yWindow="0" windowWidth="25040" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,21 +21,24 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="103">
   <si>
-    <t>subject ID</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
-    <t>control/player</t>
+    <t>player</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>subjectID</t>
+  </si>
+  <si>
+    <t>groupID</t>
   </si>
   <si>
     <t>01408</t>
   </si>
   <si>
-    <t>player</t>
-  </si>
-  <si>
     <t>01409</t>
   </si>
   <si>
@@ -133,9 +136,6 @@
   </si>
   <si>
     <t>01480</t>
-  </si>
-  <si>
-    <t>control</t>
   </si>
   <si>
     <t>01482</t>
@@ -343,20 +343,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -378,11 +384,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -405,39 +411,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,1098 +780,1098 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C99"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>68</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>40</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>58</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>63</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>48</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>55</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>62</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>60</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>46</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>48</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>54</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="4">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>61</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="4">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
         <v>47</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="4">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
         <v>57</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="4">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
         <v>55</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="4">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
         <v>54</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="4">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="4">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>65</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="4">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>50</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="4">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
         <v>63</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="4">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>57</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="4">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
         <v>69</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="4">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
         <v>63</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="4">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
         <v>56</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="4">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27">
         <v>53</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="4">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
         <v>46</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="4">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29">
         <v>47</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="4">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30">
         <v>40</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="4">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31">
         <v>41</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="4">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32">
         <v>62</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="4">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33">
         <v>42</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="4">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34">
         <v>49</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="6">
+      <c r="A35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35">
         <v>45</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36">
         <v>50</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37">
         <v>61</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38">
         <v>58</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39">
         <v>57</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40">
         <v>56</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41">
         <v>57</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42">
         <v>64</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43">
         <v>42</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44">
         <v>55</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45">
         <v>61</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46">
         <v>50</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47">
         <v>68</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48">
         <v>49</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49">
         <v>59</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50">
         <v>52</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51">
         <v>56</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52">
         <v>56</v>
       </c>
-      <c r="C52" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53">
         <v>69</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54">
         <v>56</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55">
         <v>49</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56">
         <v>41</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57">
         <v>65</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58">
         <v>42</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59">
         <v>48</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60">
         <v>62</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61">
         <v>66</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62">
         <v>53</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63">
         <v>48</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64">
         <v>57</v>
       </c>
-      <c r="C64" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65">
         <v>52</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66">
         <v>68</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67">
         <v>54</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68">
         <v>57</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69">
         <v>56</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70">
         <v>62</v>
       </c>
-      <c r="C70" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71">
         <v>68</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72">
         <v>48</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73">
         <v>52</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="10">
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74">
         <v>41</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B75" s="10">
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75">
         <v>67</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B76" s="10">
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76">
         <v>48</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77">
         <v>58</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B78" s="10">
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78">
         <v>63</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="10">
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79">
         <v>54</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80">
         <v>63</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B81" s="10">
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81">
         <v>56</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82">
         <v>40</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83">
         <v>60</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B84" s="10">
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84">
         <v>64</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B85" s="10">
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85">
         <v>59</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="10">
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86">
         <v>55</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87">
         <v>65</v>
       </c>
-      <c r="C87" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B88" s="11">
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88">
         <v>60</v>
       </c>
-      <c r="C88" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B89" s="11">
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89">
         <v>49</v>
       </c>
-      <c r="C89" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="11">
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90">
         <v>49</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="10">
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91">
         <v>57</v>
       </c>
-      <c r="C91" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B92" s="11">
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92">
         <v>47</v>
       </c>
-      <c r="C92" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B93" s="11">
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93">
         <v>61</v>
       </c>
-      <c r="C93" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B94" s="11">
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94">
         <v>53</v>
       </c>
-      <c r="C94" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B95" s="11">
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95">
         <v>63</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B96" s="10">
+      <c r="B96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96">
         <v>68</v>
       </c>
-      <c r="C96" s="8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B97" s="11">
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97">
         <v>61</v>
       </c>
-      <c r="C97" s="9" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B98" s="11">
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98">
         <v>55</v>
       </c>
-      <c r="C98" s="9" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="13" t="s">
+      <c r="A99" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B99" s="11">
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+      <c r="C99">
         <v>60</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>